<commit_message>
working csv, xls, xlsx import, rowwise and columnwise, checking for empty cells
</commit_message>
<xml_diff>
--- a/inputrow.xlsx
+++ b/inputrow.xlsx
@@ -131,13 +131,10 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -158,9 +155,6 @@
       <c r="F1" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="G1" s="0" t="n">
-        <v>2</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -198,9 +192,6 @@
       <c r="D3" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="E3" s="0" t="n">
-        <v>3</v>
-      </c>
       <c r="F3" s="0" t="n">
         <v>3</v>
       </c>
@@ -226,9 +217,6 @@
       </c>
       <c r="F4" s="0" t="n">
         <v>4</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified for xls export and central parameter settings
</commit_message>
<xml_diff>
--- a/inputrow.xlsx
+++ b/inputrow.xlsx
@@ -20,18 +20,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>WTY</t>
   </si>
   <si>
-    <t>WTYSO</t>
+    <t>WTSO</t>
+  </si>
+  <si>
+    <t>WTTO</t>
+  </si>
+  <si>
+    <t>WTRO</t>
   </si>
   <si>
     <t>MKOY</t>
   </si>
   <si>
     <t>MKOSO</t>
+  </si>
+  <si>
+    <t>MKOTO</t>
+  </si>
+  <si>
+    <t>MCKY</t>
+  </si>
+  <si>
+    <t>MCKSO</t>
+  </si>
+  <si>
+    <t>MCKTO</t>
   </si>
 </sst>
 </file>
@@ -106,8 +124,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -128,94 +150,223 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F1" s="0" t="n">
+      <c r="B1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G2" s="0" t="n">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="G3" s="0" t="n">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F4" s="0" t="n">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F10" s="1" t="n">
         <v>4</v>
       </c>
     </row>

</xml_diff>